<commit_message>
atualizando mais o main
</commit_message>
<xml_diff>
--- a/src/utils/data/num_problems.xlsx
+++ b/src/utils/data/num_problems.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\Chatbot\src\utils\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91141004-5EE0-408E-9543-3B7D3CF4351D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B2BFB6-A909-4DD1-8510-BE56DEA94AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="825" windowWidth="15375" windowHeight="7785" xr2:uid="{5406DAE8-2532-4FD1-B385-6C28F27024E4}"/>
+    <workbookView xWindow="5220" yWindow="1080" windowWidth="15375" windowHeight="7785" xr2:uid="{5406DAE8-2532-4FD1-B385-6C28F27024E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D7E0485-F263-447E-AD06-3E920F277023}">
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>